<commit_message>
Swapped names of CapacityFactor for AvailabilityFactor in preparation for upgrade to NemoMod 2.0, Julia 1.10, and juliacall juliapkg
</commit_message>
<xml_diff>
--- a/ref/data_tables_and_derivations/ENERGY/energy_inputs_to_model_with_fuel_conversion_factors.xlsx
+++ b/ref/data_tables_and_derivations/ENERGY/energy_inputs_to_model_with_fuel_conversion_factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/data_tables_and_derivations/ENERGY/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/sisepuede/ref/data_tables_and_derivations/ENERGY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FA8A85-3BCC-D74B-B90F-43184F44A3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96776DEC-7A00-EB45-83B0-4B4613155A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="500" windowWidth="26300" windowHeight="20260" firstSheet="2" activeTab="5" xr2:uid="{5FFDFBED-0EDA-184B-B159-D6A0BE4DEBC4}"/>
+    <workbookView xWindow="4320" yWindow="500" windowWidth="26300" windowHeight="20260" firstSheet="4" activeTab="10" xr2:uid="{5FFDFBED-0EDA-184B-B159-D6A0BE4DEBC4}"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="654">
   <si>
     <t>IEA World Energy Balance includes production by PJ. These sheets contain information to convert PJ to tonnes and m3 to tonnes</t>
   </si>
@@ -2194,6 +2194,9 @@
   </si>
   <si>
     <t>efficiency factor</t>
+  </si>
+  <si>
+    <t>189MJ/kg hydrogen</t>
   </si>
 </sst>
 </file>
@@ -2666,32 +2669,14 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2699,13 +2684,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2714,14 +2696,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2753,17 +2756,17 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -2993,9 +2996,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3033,7 +3036,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3139,7 +3142,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3281,7 +3284,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3340,8 +3343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376CCDCF-BF68-B44A-A3EA-06F3A7228FFF}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="A12" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3355,21 +3358,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -3493,7 +3496,10 @@
       <c r="G11" s="79"/>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
+      <c r="A12" s="28">
+        <f>52.5*3.6</f>
+        <v>189</v>
+      </c>
       <c r="B12" s="33">
         <f>1-$B10/B11</f>
         <v>0.27027399146358266</v>
@@ -3521,7 +3527,9 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="28" t="s">
+        <v>653</v>
+      </c>
       <c r="B13" s="32">
         <f>AVERAGE(B12:C12)</f>
         <v>0.30344335548796525</v>
@@ -3630,19 +3638,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A41" s="58" t="s">
+      <c r="A41" s="73" t="s">
         <v>314</v>
       </c>
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="58"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -3677,7 +3685,7 @@
         <f>1/8.07</f>
         <v>0.12391573729863692</v>
       </c>
-      <c r="G47" s="62" t="s">
+      <c r="G47" s="72" t="s">
         <v>289</v>
       </c>
     </row>
@@ -3696,7 +3704,7 @@
         <f>1.06*E47</f>
         <v>0.13135068153655513</v>
       </c>
-      <c r="G48" s="62"/>
+      <c r="G48" s="72"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -3713,7 +3721,7 @@
         <f>E48*1.1</f>
         <v>0.14448574969021066</v>
       </c>
-      <c r="G49" s="62"/>
+      <c r="G49" s="72"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -3729,7 +3737,7 @@
       <c r="E50">
         <v>6</v>
       </c>
-      <c r="G50" s="62"/>
+      <c r="G50" s="72"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -3940,8 +3948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F354AE3-1258-3A40-8310-3DF8834C6921}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3966,7 +3974,7 @@
       <c r="K1" s="82" t="s">
         <v>222</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="27" t="s">
         <v>156</v>
       </c>
       <c r="S1" s="82" t="s">
@@ -4064,11 +4072,11 @@
         <v>223</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:C5" si="0">1/(1-B4)</f>
+        <f>1/(1-B4)</f>
         <v>1.0050251256281406</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B5:C5" si="0">1/(1-C4)</f>
         <v>1.0416666666666667</v>
       </c>
       <c r="D5">
@@ -4460,7 +4468,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="X23">
-        <v>0.30344335548796525</v>
+        <v>0.30344335548796503</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -4549,15 +4557,23 @@
         <v>159</v>
       </c>
       <c r="C26">
-        <f>ROUND((B$25-1)/(D$25-1),3)</f>
-        <v>0.151</v>
+        <f>(B$25-1)/(D$25-1)</f>
+        <v>0.1514814299624424</v>
       </c>
       <c r="D26">
-        <f>ROUND((C$25-1)/(D$25-1),3)</f>
-        <v>3.5739999999999998</v>
+        <f>(C$25-1)/(D$25-1)</f>
+        <v>3.5738396624472566</v>
       </c>
       <c r="E26">
         <f>($D$25-1)*N3</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>C26*E26</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>D26*E26</f>
         <v>0</v>
       </c>
       <c r="H26" t="s">
@@ -4589,16 +4605,24 @@
         <v>158</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:C30" si="10">ROUND((B$25-1)/(D$25-1),3)</f>
-        <v>0.151</v>
+        <f t="shared" ref="C27:C30" si="10">(B$25-1)/(D$25-1)</f>
+        <v>0.1514814299624424</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:D30" si="11">ROUND((C$25-1)/(D$25-1),3)</f>
-        <v>3.5739999999999998</v>
+        <f t="shared" ref="D27:D30" si="11">(C$25-1)/(D$25-1)</f>
+        <v>3.5738396624472566</v>
       </c>
       <c r="E27">
         <f t="shared" ref="E27:E30" si="12">($D$25-1)*N4</f>
         <v>0.32644628099173556</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F30" si="13">C27*E27</f>
+        <v>4.9450549450549386E-2</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ref="G27:G30" si="14">D27*E27</f>
+        <v>1.1666666666666665</v>
       </c>
       <c r="O27" s="23" t="s">
         <v>239</v>
@@ -4627,15 +4651,23 @@
       </c>
       <c r="C28">
         <f t="shared" si="10"/>
-        <v>0.151</v>
+        <v>0.1514814299624424</v>
       </c>
       <c r="D28">
         <f t="shared" si="11"/>
-        <v>3.5739999999999998</v>
+        <v>3.5738396624472566</v>
       </c>
       <c r="E28">
         <f t="shared" si="12"/>
         <v>0.30724355858045699</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="13"/>
+        <v>4.6541693600517069E-2</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="14"/>
+        <v>1.0980392156862744</v>
       </c>
       <c r="O28" s="23" t="s">
         <v>239</v>
@@ -4664,15 +4696,23 @@
       </c>
       <c r="C29">
         <f t="shared" si="10"/>
-        <v>0.151</v>
+        <v>0.1514814299624424</v>
       </c>
       <c r="D29">
         <f t="shared" si="11"/>
-        <v>3.5739999999999998</v>
+        <v>3.5738396624472566</v>
       </c>
       <c r="E29">
         <f t="shared" si="12"/>
         <v>1.9202722411278562E-2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="13"/>
+        <v>2.9088558500323168E-3</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="14"/>
+        <v>6.8627450980392149E-2</v>
       </c>
       <c r="O29" s="23" t="s">
         <v>239</v>
@@ -4701,14 +4741,22 @@
       </c>
       <c r="C30">
         <f t="shared" si="10"/>
-        <v>0.151</v>
+        <v>0.1514814299624424</v>
       </c>
       <c r="D30">
         <f t="shared" si="11"/>
-        <v>3.5739999999999998</v>
+        <v>3.5738396624472566</v>
       </c>
       <c r="E30">
         <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O30" s="23" t="s">
@@ -4855,11 +4903,11 @@
         <v>223</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:C35" si="13">1/(1-B34)</f>
+        <f t="shared" ref="B35:C35" si="15">1/(1-B34)</f>
         <v>1.0416666666666667</v>
       </c>
       <c r="C35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.1235955056179776</v>
       </c>
       <c r="D35">
@@ -4935,11 +4983,11 @@
         <v>158</v>
       </c>
       <c r="C37">
-        <f t="shared" ref="C37:C40" si="14">ROUND((B$35-1)/(D$35-1),3)</f>
+        <f t="shared" ref="C37:C40" si="16">ROUND((B$35-1)/(D$35-1),3)</f>
         <v>0.51400000000000001</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:D40" si="15">ROUND((C$35-1)/(D$35-1),3)</f>
+        <f t="shared" ref="D37:D40" si="17">ROUND((C$35-1)/(D$35-1),3)</f>
         <v>1.524</v>
       </c>
       <c r="E37">
@@ -4973,11 +5021,11 @@
         <v>160</v>
       </c>
       <c r="C38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.51400000000000001</v>
       </c>
       <c r="D38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.524</v>
       </c>
       <c r="E38">
@@ -4985,7 +5033,7 @@
         <v>3.8155802861685136E-2</v>
       </c>
       <c r="G38">
-        <f t="shared" ref="G38:G39" si="16">1/E38</f>
+        <f t="shared" ref="G38:G39" si="18">1/E38</f>
         <v>26.208333333333389</v>
       </c>
       <c r="O38" s="23" t="s">
@@ -5007,11 +5055,11 @@
         <v>161</v>
       </c>
       <c r="C39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.51400000000000001</v>
       </c>
       <c r="D39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.524</v>
       </c>
       <c r="E39">
@@ -5019,7 +5067,7 @@
         <v>2.384737678855321E-3</v>
       </c>
       <c r="G39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>419.33333333333422</v>
       </c>
       <c r="O39" s="23" t="s">
@@ -5041,11 +5089,11 @@
         <v>162</v>
       </c>
       <c r="C40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.51400000000000001</v>
       </c>
       <c r="D40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.524</v>
       </c>
       <c r="E40">
@@ -5453,6 +5501,7 @@
     <hyperlink ref="H14" r:id="rId2" xr:uid="{A0D96530-342C-1349-BA17-1F0D5520F2CB}"/>
     <hyperlink ref="E34" r:id="rId3" xr:uid="{F5858204-8F43-9A46-8BAC-BC1155CA186B}"/>
     <hyperlink ref="H24" r:id="rId4" xr:uid="{B782A8F5-F8B6-714D-9879-4BFACD35A4B7}"/>
+    <hyperlink ref="L1" r:id="rId5" xr:uid="{9960542F-E14A-054A-92F5-889FD9C91A48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5475,7 +5524,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>190</v>
       </c>
       <c r="B1" t="s">
@@ -5505,7 +5554,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="63"/>
+      <c r="A2" s="64"/>
       <c r="B2" t="s">
         <v>189</v>
       </c>
@@ -5526,7 +5575,7 @@
       <c r="S2" s="36"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="63"/>
+      <c r="A3" s="64"/>
       <c r="B3" t="s">
         <v>162</v>
       </c>
@@ -5981,14 +6030,14 @@
       <c r="S29" s="36"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G30" s="62" t="s">
+      <c r="G30" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="H30" s="62"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
       <c r="N30" s="36"/>
       <c r="O30" s="36"/>
       <c r="P30" s="36"/>
@@ -6021,14 +6070,14 @@
       <c r="S33" s="36"/>
     </row>
     <row r="34" spans="14:19" x14ac:dyDescent="0.2">
-      <c r="N34" s="62" t="s">
+      <c r="N34" s="72" t="s">
         <v>191</v>
       </c>
-      <c r="O34" s="62"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="62"/>
-      <c r="R34" s="62"/>
-      <c r="S34" s="62"/>
+      <c r="O34" s="72"/>
+      <c r="P34" s="72"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="72"/>
+      <c r="S34" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7392,32 +7441,32 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="87" t="s">
         <v>504</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
     </row>
     <row r="17" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="88" t="s">
         <v>504</v>
       </c>
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="88"/>
     </row>
     <row r="18" spans="1:11" ht="26" x14ac:dyDescent="0.3">
       <c r="A18" s="47"/>
@@ -7432,25 +7481,25 @@
       <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:11" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="87" t="s">
+      <c r="A19" s="89" t="s">
         <v>506</v>
       </c>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="88"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
     </row>
     <row r="21" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="61" t="s">
+      <c r="A21" s="67" t="s">
         <v>495</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
       <c r="K21">
         <f>47951850/5462141</f>
         <v>8.7789476690550465</v>
@@ -7570,17 +7619,17 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="87" t="s">
+      <c r="A39" s="89" t="s">
         <v>507</v>
       </c>
-      <c r="B39" s="88"/>
-      <c r="C39" s="88"/>
-      <c r="D39" s="88"/>
-      <c r="E39" s="88"/>
-      <c r="F39" s="88"/>
-      <c r="G39" s="88"/>
-      <c r="H39" s="88"/>
-      <c r="I39" s="88"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="90"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="90"/>
+      <c r="I39" s="90"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -7656,18 +7705,18 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="A52" s="89" t="s">
+      <c r="A52" s="88" t="s">
         <v>535</v>
       </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="89"/>
-      <c r="D52" s="89"/>
-      <c r="E52" s="89"/>
-      <c r="F52" s="89"/>
-      <c r="G52" s="89"/>
-      <c r="H52" s="89"/>
-      <c r="I52" s="89"/>
-      <c r="J52" s="89"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="88"/>
+      <c r="D52" s="88"/>
+      <c r="E52" s="88"/>
+      <c r="F52" s="88"/>
+      <c r="G52" s="88"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="88"/>
     </row>
     <row r="53" spans="1:10" ht="26" x14ac:dyDescent="0.3">
       <c r="A53" s="47"/>
@@ -7682,17 +7731,17 @@
       <c r="J53" s="47"/>
     </row>
     <row r="54" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="87" t="s">
+      <c r="A54" s="89" t="s">
         <v>507</v>
       </c>
-      <c r="B54" s="88"/>
-      <c r="C54" s="88"/>
-      <c r="D54" s="88"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="88"/>
-      <c r="G54" s="88"/>
-      <c r="H54" s="88"/>
-      <c r="I54" s="88"/>
+      <c r="B54" s="90"/>
+      <c r="C54" s="90"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="90"/>
+      <c r="F54" s="90"/>
+      <c r="G54" s="90"/>
+      <c r="H54" s="90"/>
+      <c r="I54" s="90"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -7841,16 +7890,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="A52:J52"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="C57:C58"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="C25:C29"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A17:J17"/>
     <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="A52:J52"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="C57:C58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8599,18 +8648,18 @@
   </cols>
   <sheetData>
     <row r="9" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="88" t="s">
         <v>514</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
     </row>
     <row r="10" spans="1:10" ht="26" x14ac:dyDescent="0.3">
       <c r="A10" s="47"/>
@@ -8625,17 +8674,17 @@
       <c r="J10" s="47"/>
     </row>
     <row r="11" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="89" t="s">
         <v>515</v>
       </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -8677,11 +8726,11 @@
       <c r="D18" t="s">
         <v>523</v>
       </c>
-      <c r="M18" s="60" t="s">
+      <c r="M18" s="76" t="s">
         <v>521</v>
       </c>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
+      <c r="N18" s="76"/>
+      <c r="O18" s="76"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C19">
@@ -8693,9 +8742,9 @@
       <c r="E19" t="s">
         <v>524</v>
       </c>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="60"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="76"/>
+      <c r="O19" s="76"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C20">
@@ -8707,9 +8756,9 @@
       <c r="E20" t="s">
         <v>525</v>
       </c>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="60"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="76"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C21">
@@ -8923,19 +8972,19 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
       <c r="L11" t="s">
         <v>90</v>
       </c>
@@ -8959,42 +9008,42 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="61"/>
-      <c r="S15" s="61"/>
-      <c r="T15" s="61"/>
-      <c r="U15" s="61"/>
-      <c r="V15" s="61"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="67"/>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="67"/>
+      <c r="S15" s="67"/>
+      <c r="T15" s="67"/>
+      <c r="U15" s="67"/>
+      <c r="V15" s="67"/>
     </row>
     <row r="16" spans="1:22" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="72"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="66"/>
-      <c r="S16" s="66"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="68"/>
+      <c r="Q16" s="68"/>
+      <c r="R16" s="68"/>
+      <c r="S16" s="68"/>
       <c r="T16" s="18"/>
       <c r="U16" s="18"/>
     </row>
@@ -9041,7 +9090,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="64" t="s">
         <v>88</v>
       </c>
       <c r="B18" t="s">
@@ -9095,7 +9144,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
+      <c r="A19" s="64"/>
       <c r="B19" t="s">
         <v>36</v>
       </c>
@@ -9147,7 +9196,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
+      <c r="A20" s="64"/>
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -9199,7 +9248,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="8" t="s">
         <v>85</v>
       </c>
@@ -9248,7 +9297,7 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="8" t="s">
         <v>86</v>
       </c>
@@ -9279,7 +9328,7 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="8" t="s">
         <v>87</v>
       </c>
@@ -9311,7 +9360,7 @@
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="63"/>
+      <c r="A24" s="64"/>
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -9335,7 +9384,7 @@
       <c r="A25" s="20"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="64" t="s">
         <v>89</v>
       </c>
       <c r="B26" t="s">
@@ -9358,7 +9407,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
+      <c r="A27" s="64"/>
       <c r="B27" t="s">
         <v>91</v>
       </c>
@@ -9385,10 +9434,10 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C28" s="8"/>
-      <c r="N28" s="62"/>
-      <c r="O28" s="62"/>
-      <c r="P28" s="62"/>
-      <c r="Q28" s="62"/>
+      <c r="N28" s="72"/>
+      <c r="O28" s="72"/>
+      <c r="P28" s="72"/>
+      <c r="Q28" s="72"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C29" s="8"/>
@@ -9406,13 +9455,13 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J30" s="65" t="s">
+      <c r="J30" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="67" t="s">
+      <c r="K30" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="68"/>
+      <c r="L30" s="62"/>
       <c r="M30" s="69"/>
       <c r="N30" s="9">
         <v>7.0000000000000007E-2</v>
@@ -9428,12 +9477,12 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J31" s="65"/>
-      <c r="K31" s="70" t="s">
+      <c r="J31" s="74"/>
+      <c r="K31" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="63"/>
-      <c r="M31" s="71"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="70"/>
       <c r="N31" s="12">
         <v>0.83</v>
       </c>
@@ -9452,12 +9501,12 @@
         <f>(0.0022*0.037)^0.5</f>
         <v>9.0221948549119683E-3</v>
       </c>
-      <c r="J32" s="65"/>
-      <c r="K32" s="72" t="s">
+      <c r="J32" s="74"/>
+      <c r="K32" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="L32" s="73"/>
-      <c r="M32" s="74"/>
+      <c r="L32" s="66"/>
+      <c r="M32" s="71"/>
       <c r="N32" s="14">
         <v>0.1</v>
       </c>
@@ -9472,13 +9521,13 @@
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J33" s="64" t="s">
+      <c r="J33" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="K33" s="67" t="s">
+      <c r="K33" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="L33" s="68"/>
+      <c r="L33" s="62"/>
       <c r="M33" s="69"/>
       <c r="N33" s="9">
         <v>0.09</v>
@@ -9494,12 +9543,12 @@
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J34" s="64"/>
-      <c r="K34" s="70" t="s">
+      <c r="J34" s="60"/>
+      <c r="K34" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="L34" s="63"/>
-      <c r="M34" s="71"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="70"/>
       <c r="N34" s="12">
         <v>0.78</v>
       </c>
@@ -9514,12 +9563,12 @@
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J35" s="64"/>
-      <c r="K35" s="72" t="s">
+      <c r="J35" s="60"/>
+      <c r="K35" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="L35" s="73"/>
-      <c r="M35" s="74"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="71"/>
       <c r="N35" s="14">
         <v>0.13</v>
       </c>
@@ -9534,13 +9583,13 @@
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J36" s="64" t="s">
+      <c r="J36" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="K36" s="67" t="s">
+      <c r="K36" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="L36" s="68"/>
+      <c r="L36" s="62"/>
       <c r="M36" s="69"/>
       <c r="N36" s="9">
         <v>0.2</v>
@@ -9556,12 +9605,12 @@
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J37" s="64"/>
-      <c r="K37" s="70" t="s">
+      <c r="J37" s="60"/>
+      <c r="K37" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="63"/>
-      <c r="M37" s="71"/>
+      <c r="L37" s="64"/>
+      <c r="M37" s="70"/>
       <c r="N37" s="12">
         <v>0.8</v>
       </c>
@@ -9576,12 +9625,12 @@
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J38" s="64"/>
-      <c r="K38" s="72" t="s">
+      <c r="J38" s="60"/>
+      <c r="K38" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="L38" s="73"/>
-      <c r="M38" s="74"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="71"/>
       <c r="N38" s="12">
         <v>0</v>
       </c>
@@ -9596,14 +9645,14 @@
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J39" s="64" t="s">
+      <c r="J39" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="K39" s="67" t="s">
+      <c r="K39" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="L39" s="68"/>
-      <c r="M39" s="68"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="62"/>
       <c r="N39" s="9">
         <f>AVERAGE(N30,N33,N36)</f>
         <v>0.12</v>
@@ -9622,12 +9671,12 @@
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J40" s="64"/>
-      <c r="K40" s="70" t="s">
+      <c r="J40" s="60"/>
+      <c r="K40" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="63"/>
-      <c r="M40" s="63"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="64"/>
       <c r="N40" s="12">
         <f t="shared" ref="N40:Q41" si="5">AVERAGE(N31,N34,N37)</f>
         <v>0.80333333333333334</v>
@@ -9646,12 +9695,12 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J41" s="64"/>
-      <c r="K41" s="72" t="s">
+      <c r="J41" s="60"/>
+      <c r="K41" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="L41" s="73"/>
-      <c r="M41" s="73"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="66"/>
       <c r="N41" s="14">
         <f t="shared" si="5"/>
         <v>7.6666666666666675E-2</v>
@@ -9698,14 +9747,14 @@
       <c r="G43" t="s">
         <v>47</v>
       </c>
-      <c r="I43" s="76" t="s">
+      <c r="I43" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="J43" s="76"/>
-      <c r="K43" s="76"/>
-      <c r="L43" s="76"/>
-      <c r="M43" s="76"/>
-      <c r="N43" s="75">
+      <c r="J43" s="59"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="59"/>
+      <c r="M43" s="59"/>
+      <c r="N43" s="58">
         <f>1-N42</f>
         <v>8.7121212121212155E-2</v>
       </c>
@@ -9730,12 +9779,12 @@
         <f>F43-F22-F23</f>
         <v>6.8000000000000027E-8</v>
       </c>
-      <c r="I44" s="76"/>
-      <c r="J44" s="76"/>
-      <c r="K44" s="76"/>
-      <c r="L44" s="76"/>
-      <c r="M44" s="76"/>
-      <c r="N44" s="75"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
+      <c r="L44" s="59"/>
+      <c r="M44" s="59"/>
+      <c r="N44" s="58"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
@@ -9852,19 +9901,19 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="58" t="s">
+      <c r="A51" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="58"/>
+      <c r="B51" s="73"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
+      <c r="E51" s="73"/>
+      <c r="F51" s="73"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="73"/>
+      <c r="I51" s="73"/>
+      <c r="J51" s="73"/>
+      <c r="K51" s="73"/>
     </row>
     <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="26" t="s">
@@ -9883,19 +9932,19 @@
     </row>
     <row r="56" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="58" t="s">
+      <c r="A57" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
-      <c r="J57" s="58"/>
-      <c r="K57" s="58"/>
+      <c r="B57" s="73"/>
+      <c r="C57" s="73"/>
+      <c r="D57" s="73"/>
+      <c r="E57" s="73"/>
+      <c r="F57" s="73"/>
+      <c r="G57" s="73"/>
+      <c r="H57" s="73"/>
+      <c r="I57" s="73"/>
+      <c r="J57" s="73"/>
+      <c r="K57" s="73"/>
     </row>
     <row r="58" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="26" t="s">
@@ -9921,34 +9970,34 @@
       </c>
     </row>
     <row r="64" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A64" s="58" t="s">
+      <c r="A64" s="73" t="s">
         <v>280</v>
       </c>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="58"/>
-      <c r="F64" s="58"/>
-      <c r="G64" s="58"/>
-      <c r="H64" s="58"/>
-      <c r="I64" s="58"/>
-      <c r="J64" s="58"/>
-      <c r="K64" s="58"/>
+      <c r="B64" s="73"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
+      <c r="F64" s="73"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="73"/>
+      <c r="I64" s="73"/>
+      <c r="J64" s="73"/>
+      <c r="K64" s="73"/>
     </row>
     <row r="71" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A71" s="58" t="s">
+      <c r="A71" s="73" t="s">
         <v>315</v>
       </c>
-      <c r="B71" s="58"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
-      <c r="F71" s="58"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="58"/>
-      <c r="I71" s="58"/>
-      <c r="J71" s="58"/>
-      <c r="K71" s="58"/>
+      <c r="B71" s="73"/>
+      <c r="C71" s="73"/>
+      <c r="D71" s="73"/>
+      <c r="E71" s="73"/>
+      <c r="F71" s="73"/>
+      <c r="G71" s="73"/>
+      <c r="H71" s="73"/>
+      <c r="I71" s="73"/>
+      <c r="J71" s="73"/>
+      <c r="K71" s="73"/>
     </row>
     <row r="72" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="26" t="s">
@@ -9961,10 +10010,10 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="59" t="s">
+      <c r="A74" s="75" t="s">
         <v>309</v>
       </c>
-      <c r="B74" s="59"/>
+      <c r="B74" s="75"/>
       <c r="C74" s="42" t="s">
         <v>109</v>
       </c>
@@ -9989,10 +10038,10 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="59" t="s">
+      <c r="A76" s="75" t="s">
         <v>317</v>
       </c>
-      <c r="B76" s="59"/>
+      <c r="B76" s="75"/>
       <c r="C76" s="41">
         <f>C75*$B$80</f>
         <v>2.6086956521739112E-4</v>
@@ -10063,12 +10112,21 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="N43:N44"/>
-    <mergeCell ref="I43:M44"/>
-    <mergeCell ref="J39:J41"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="A64:K64"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="J36:J38"/>
+    <mergeCell ref="J33:J35"/>
+    <mergeCell ref="J30:J32"/>
     <mergeCell ref="N15:V15"/>
     <mergeCell ref="R16:S16"/>
     <mergeCell ref="K36:M36"/>
@@ -10082,21 +10140,12 @@
     <mergeCell ref="N28:Q28"/>
     <mergeCell ref="K34:M34"/>
     <mergeCell ref="K35:M35"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="J36:J38"/>
-    <mergeCell ref="J33:J35"/>
-    <mergeCell ref="J30:J32"/>
-    <mergeCell ref="A71:K71"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="A64:K64"/>
-    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="I43:M44"/>
+    <mergeCell ref="J39:J41"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="K41:M41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A55" r:id="rId1" xr:uid="{939BE22A-9CE0-E745-AEFB-468D46C49282}"/>
@@ -10361,31 +10410,31 @@
       <c r="N5" s="44"/>
     </row>
     <row r="6" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
       <c r="L6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
@@ -10415,7 +10464,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="64" t="s">
         <v>88</v>
       </c>
       <c r="B9" t="s">
@@ -10457,7 +10506,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
+      <c r="A10" s="64"/>
       <c r="B10" t="s">
         <v>122</v>
       </c>
@@ -10501,7 +10550,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
+      <c r="A11" s="64"/>
       <c r="B11" t="s">
         <v>123</v>
       </c>
@@ -10541,7 +10590,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
+      <c r="A12" s="64"/>
       <c r="B12" t="s">
         <v>124</v>
       </c>
@@ -10585,7 +10634,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
+      <c r="A13" s="64"/>
       <c r="B13" t="s">
         <v>125</v>
       </c>
@@ -10607,7 +10656,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="64" t="s">
         <v>89</v>
       </c>
       <c r="B14" t="s">
@@ -10645,7 +10694,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
+      <c r="A15" s="64"/>
       <c r="B15" t="s">
         <v>129</v>
       </c>
@@ -10681,7 +10730,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
+      <c r="A16" s="64"/>
       <c r="B16" t="s">
         <v>126</v>
       </c>
@@ -10717,7 +10766,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
+      <c r="A17" s="64"/>
       <c r="B17" t="s">
         <v>127</v>
       </c>
@@ -10754,19 +10803,19 @@
     </row>
     <row r="18" spans="1:15" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="73" t="s">
         <v>303</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
@@ -10894,10 +10943,10 @@
       <c r="B34">
         <v>408.31599999999997</v>
       </c>
-      <c r="D34" s="59" t="s">
+      <c r="D34" s="75" t="s">
         <v>309</v>
       </c>
-      <c r="E34" s="59"/>
+      <c r="E34" s="75"/>
       <c r="F34" s="42" t="s">
         <v>109</v>
       </c>
@@ -10938,10 +10987,10 @@
         <f>B34/B35</f>
         <v>1.6789999588798881E-2</v>
       </c>
-      <c r="D36" s="59" t="s">
+      <c r="D36" s="75" t="s">
         <v>313</v>
       </c>
-      <c r="E36" s="59"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="41">
         <f>F35*B36</f>
         <v>3.3579999177597762E-5</v>
@@ -10986,19 +11035,19 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="58" t="s">
+      <c r="A40" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="58"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
@@ -11046,7 +11095,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11109,8 +11158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4649CCF-D008-C24D-A313-269ECCCA33E0}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11519,34 +11568,34 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G16" s="62" t="s">
+      <c r="G16" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="N16" s="62" t="s">
+      <c r="H16" s="72"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="72"/>
+      <c r="N16" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="72"/>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
       <c r="U16" s="23"/>
@@ -12151,19 +12200,19 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="26"/>
@@ -12173,19 +12222,19 @@
     </row>
     <row r="39" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="58" t="s">
+      <c r="A40" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="58"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="26"/>

</xml_diff>